<commit_message>
Adding notes to micromadness and hex tools
</commit_message>
<xml_diff>
--- a/Ch3_Hardware/MicroMadnessTournament.xlsx
+++ b/Ch3_Hardware/MicroMadnessTournament.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eleci\work\oreilly\git\Ch3_Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70ACBEA9-31EF-4560-A411-2315B6F8B227}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC97CE17-F7EA-423E-9226-A55071B2067D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="19380" windowHeight="20970" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Contenders" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="180">
   <si>
     <t xml:space="preserve">Board </t>
   </si>
@@ -291,9 +291,6 @@
   </si>
   <si>
     <t>Snekboard</t>
-  </si>
-  <si>
-    <t>Tinkersphere DIY Pocket Oscilloscope Kit</t>
   </si>
   <si>
     <t>NK-BEDM487</t>
@@ -1066,58 +1063,58 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1890,8 +1887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{704D91A8-9203-42B4-AABB-078766894F94}">
   <dimension ref="A1:D120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C104" sqref="C104"/>
+    <sheetView topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="B102" sqref="B102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
@@ -1903,17 +1900,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="13">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="80" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="102" t="s">
+      <c r="B1" s="80" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="102" t="s">
+      <c r="C1" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="102" t="s">
-        <v>129</v>
+      <c r="D1" s="80" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1922,28 +1919,28 @@
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="B3" s="103" t="s">
-        <v>176</v>
+      <c r="B3" s="81" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="B4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="B5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="B6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="B7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1952,8 +1949,8 @@
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="B9" s="103" t="s">
-        <v>180</v>
+      <c r="B9" s="81" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1963,12 +1960,12 @@
     </row>
     <row r="11" spans="1:4">
       <c r="B11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="B12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1978,42 +1975,42 @@
     </row>
     <row r="14" spans="1:4">
       <c r="B14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="B15" s="103" t="s">
-        <v>175</v>
+      <c r="B15" s="81" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="B16" s="103" t="s">
-        <v>174</v>
+      <c r="B16" s="81" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="17" spans="2:2">
       <c r="B17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="18" spans="2:2">
       <c r="B18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19" spans="2:2">
       <c r="B19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="20" spans="2:2">
-      <c r="B20" s="103" t="s">
-        <v>173</v>
+      <c r="B20" s="81" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="21" spans="2:2">
-      <c r="B21" s="103" t="s">
-        <v>172</v>
+      <c r="B21" s="81" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="22" spans="2:2">
@@ -2022,108 +2019,108 @@
       </c>
     </row>
     <row r="23" spans="2:2">
-      <c r="B23" s="104" t="s">
-        <v>179</v>
+      <c r="B23" s="82" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="24" spans="2:2">
-      <c r="B24" s="103" t="s">
-        <v>178</v>
+      <c r="B24" s="81" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="25" spans="2:2">
-      <c r="B25" s="103" t="s">
-        <v>177</v>
+      <c r="B25" s="81" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="26" spans="2:2">
       <c r="B26" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="27" spans="2:2">
-      <c r="B27" s="103" t="s">
-        <v>171</v>
+      <c r="B27" s="81" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="28" spans="2:2">
-      <c r="B28" s="103" t="s">
-        <v>170</v>
+      <c r="B28" s="81" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="29" spans="2:2">
       <c r="B29" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="30" spans="2:2">
       <c r="B30" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="31" spans="2:2">
-      <c r="B31" s="103" t="s">
-        <v>169</v>
+      <c r="B31" s="81" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="32" spans="2:2">
       <c r="B32" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="33" spans="2:2">
       <c r="B33" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="34" spans="2:2">
-      <c r="B34" s="103" t="s">
-        <v>123</v>
+      <c r="B34" s="81" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="35" spans="2:2">
-      <c r="B35" s="103" t="s">
-        <v>168</v>
+      <c r="B35" s="81" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="36" spans="2:2">
       <c r="B36" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="37" spans="2:2">
-      <c r="B37" s="103" t="s">
-        <v>167</v>
+      <c r="B37" s="81" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="38" spans="2:2">
       <c r="B38" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="39" spans="2:2">
       <c r="B39" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="40" spans="2:2">
       <c r="B40" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="41" spans="2:2">
       <c r="B41" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="42" spans="2:2">
-      <c r="B42" s="103" t="s">
-        <v>166</v>
+      <c r="B42" s="81" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="43" spans="2:2">
-      <c r="B43" s="103" t="s">
-        <v>165</v>
+      <c r="B43" s="81" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="44" spans="2:2">
@@ -2133,52 +2130,52 @@
     </row>
     <row r="45" spans="2:2">
       <c r="B45" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="46" spans="2:2">
       <c r="B46" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="47" spans="2:2">
-      <c r="B47" s="103" t="s">
-        <v>164</v>
+      <c r="B47" s="81" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="48" spans="2:2">
-      <c r="B48" s="104" t="s">
-        <v>163</v>
+      <c r="B48" s="82" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="49" spans="2:2">
       <c r="B49" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="50" spans="2:2">
       <c r="B50" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="51" spans="2:2">
       <c r="B51" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="52" spans="2:2">
-      <c r="B52" s="103" t="s">
-        <v>162</v>
+      <c r="B52" s="81" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="53" spans="2:2">
       <c r="B53" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="54" spans="2:2">
       <c r="B54" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="55" spans="2:2">
@@ -2187,28 +2184,28 @@
       </c>
     </row>
     <row r="56" spans="2:2">
-      <c r="B56" s="103" t="s">
-        <v>161</v>
+      <c r="B56" s="81" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="57" spans="2:2">
-      <c r="B57" s="103" t="s">
-        <v>160</v>
+      <c r="B57" s="81" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="58" spans="2:2">
-      <c r="B58" s="103" t="s">
-        <v>159</v>
+      <c r="B58" s="81" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="59" spans="2:2">
-      <c r="B59" s="103" t="s">
-        <v>158</v>
+      <c r="B59" s="81" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="60" spans="2:2">
       <c r="B60" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="61" spans="2:2">
@@ -2218,274 +2215,272 @@
     </row>
     <row r="62" spans="2:2">
       <c r="B62" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="63" spans="2:2">
       <c r="B63" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="64" spans="2:2">
+      <c r="B64" s="81" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2">
+      <c r="B65" s="81" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2">
+      <c r="B66" s="81" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2">
+      <c r="B67" s="81" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="68" spans="2:2">
+      <c r="B68" s="81" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="69" spans="2:2">
+      <c r="B69" s="81" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="70" spans="2:2">
+      <c r="B70" s="81" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="71" spans="2:2">
+      <c r="B71" s="81" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="72" spans="2:2">
+      <c r="B72" s="81" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="73" spans="2:2">
+      <c r="B73" s="81" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="74" spans="2:2">
+      <c r="B74" s="81" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="75" spans="2:2">
+      <c r="B75" s="81" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="76" spans="2:2">
+      <c r="B76" s="81" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="77" spans="2:2">
+      <c r="B77" s="81" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="64" spans="2:2">
-      <c r="B64" s="103" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="65" spans="2:2">
-      <c r="B65" s="103" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="66" spans="2:2">
-      <c r="B66" s="103" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="67" spans="2:2">
-      <c r="B67" s="103" t="s">
+    <row r="78" spans="2:2">
+      <c r="B78" s="81" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="79" spans="2:2">
+      <c r="B79" s="81" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="80" spans="2:2">
+      <c r="B80" s="81" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2">
+      <c r="B81" s="81" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="82" spans="2:2">
+      <c r="B82" s="81" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="83" spans="2:2">
+      <c r="B83" s="81" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="84" spans="2:2">
+      <c r="B84" s="81" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="85" spans="2:2">
+      <c r="B85" s="81" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="86" spans="2:2">
+      <c r="B86" s="81" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="87" spans="2:2">
+      <c r="B87" s="81" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="88" spans="2:2">
+      <c r="B88" s="81" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="89" spans="2:2">
+      <c r="B89" s="81" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="90" spans="2:2">
+      <c r="B90" s="81" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="91" spans="2:2">
+      <c r="B91" s="81" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="92" spans="2:2">
+      <c r="B92" s="81" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="93" spans="2:2">
+      <c r="B93" s="81" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="94" spans="2:2">
+      <c r="B94" s="81" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="95" spans="2:2">
+      <c r="B95" s="81" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="96" spans="2:2">
+      <c r="B96" s="81" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="97" spans="2:2">
+      <c r="B97" s="81" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="98" spans="2:2">
+      <c r="B98" s="81" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="99" spans="2:2">
+      <c r="B99" s="81" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="100" spans="2:2">
+      <c r="B100" s="81" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="101" spans="2:2">
+      <c r="B101" s="81"/>
+    </row>
+    <row r="102" spans="2:2">
+      <c r="B102" s="81" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="103" spans="2:2">
+      <c r="B103" s="81" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="68" spans="2:2">
-      <c r="B68" s="103" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="69" spans="2:2">
-      <c r="B69" s="103" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="70" spans="2:2">
-      <c r="B70" s="103" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="71" spans="2:2">
-      <c r="B71" s="103" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="72" spans="2:2">
-      <c r="B72" s="103" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="73" spans="2:2">
-      <c r="B73" s="103" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="74" spans="2:2">
-      <c r="B74" s="103" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="75" spans="2:2">
-      <c r="B75" s="103" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="76" spans="2:2">
-      <c r="B76" s="103" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="77" spans="2:2">
-      <c r="B77" s="103" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="78" spans="2:2">
-      <c r="B78" s="103" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="79" spans="2:2">
-      <c r="B79" s="103" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="80" spans="2:2">
-      <c r="B80" s="103" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="81" spans="2:2">
-      <c r="B81" s="103" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="82" spans="2:2">
-      <c r="B82" s="103" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="83" spans="2:2">
-      <c r="B83" s="103" t="s">
+    <row r="104" spans="2:2">
+      <c r="B104" s="81" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="105" spans="2:2">
+      <c r="B105" s="81" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="84" spans="2:2">
-      <c r="B84" s="103" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="85" spans="2:2">
-      <c r="B85" s="103" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="86" spans="2:2">
-      <c r="B86" s="103" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="87" spans="2:2">
-      <c r="B87" s="103" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="88" spans="2:2">
-      <c r="B88" s="103" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="89" spans="2:2">
-      <c r="B89" s="103" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="90" spans="2:2">
-      <c r="B90" s="103" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="91" spans="2:2">
-      <c r="B91" s="103" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="92" spans="2:2">
-      <c r="B92" s="103" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="93" spans="2:2">
-      <c r="B93" s="103" t="s">
+    <row r="106" spans="2:2">
+      <c r="B106" s="81" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="107" spans="2:2">
+      <c r="B107" s="81" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="108" spans="2:2">
+      <c r="B108" s="81" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="94" spans="2:2">
-      <c r="B94" s="103" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="95" spans="2:2">
-      <c r="B95" s="103" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="96" spans="2:2">
-      <c r="B96" s="103" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="97" spans="2:2">
-      <c r="B97" s="103" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="98" spans="2:2">
-      <c r="B98" s="103" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="99" spans="2:2">
-      <c r="B99" s="103" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="100" spans="2:2">
-      <c r="B100" s="103" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="101" spans="2:2">
-      <c r="B101" s="103" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="102" spans="2:2">
-      <c r="B102" s="103" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="103" spans="2:2">
-      <c r="B103" s="103" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="104" spans="2:2">
-      <c r="B104" s="103" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="105" spans="2:2">
-      <c r="B105" s="103" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="106" spans="2:2">
-      <c r="B106" s="103" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="107" spans="2:2">
-      <c r="B107" s="103" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="108" spans="2:2">
-      <c r="B108" s="103" t="s">
-        <v>136</v>
-      </c>
-    </row>
     <row r="109" spans="2:2">
-      <c r="B109" s="103"/>
+      <c r="B109" s="81"/>
     </row>
     <row r="110" spans="2:2">
-      <c r="B110" s="103"/>
+      <c r="B110" s="81"/>
     </row>
     <row r="111" spans="2:2">
-      <c r="B111" s="103"/>
+      <c r="B111" s="81"/>
     </row>
     <row r="112" spans="2:2">
-      <c r="B112" s="103"/>
+      <c r="B112" s="81"/>
     </row>
     <row r="113" spans="2:2">
-      <c r="B113" s="103"/>
+      <c r="B113" s="81"/>
     </row>
     <row r="114" spans="2:2">
-      <c r="B114" s="103"/>
+      <c r="B114" s="81"/>
     </row>
     <row r="115" spans="2:2">
-      <c r="B115" s="103"/>
+      <c r="B115" s="81"/>
     </row>
     <row r="116" spans="2:2">
-      <c r="B116" s="103"/>
+      <c r="B116" s="81"/>
     </row>
     <row r="117" spans="2:2">
-      <c r="B117" s="103"/>
+      <c r="B117" s="81"/>
     </row>
     <row r="118" spans="2:2">
-      <c r="B118" s="103"/>
+      <c r="B118" s="81"/>
     </row>
     <row r="119" spans="2:2">
-      <c r="B119" s="103"/>
+      <c r="B119" s="81"/>
     </row>
     <row r="120" spans="2:2">
-      <c r="B120" s="103"/>
+      <c r="B120" s="81"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D996">
@@ -2503,7 +2498,9 @@
   </sheetPr>
   <dimension ref="A1:B59"/>
   <sheetViews>
-    <sheetView topLeftCell="A48" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
@@ -3124,55 +3121,55 @@
       <c r="AE1" s="21"/>
     </row>
     <row r="2" spans="1:31" ht="18" customHeight="1">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="85" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="87"/>
-      <c r="C2" s="87"/>
-      <c r="D2" s="86" t="s">
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="85" t="s">
         <v>64</v>
       </c>
-      <c r="E2" s="87"/>
-      <c r="F2" s="87"/>
-      <c r="G2" s="86" t="s">
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="85" t="s">
         <v>65</v>
       </c>
-      <c r="H2" s="87"/>
-      <c r="I2" s="87"/>
-      <c r="J2" s="86" t="s">
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="85" t="s">
         <v>66</v>
       </c>
-      <c r="K2" s="87"/>
-      <c r="L2" s="99"/>
+      <c r="K2" s="86"/>
+      <c r="L2" s="87"/>
       <c r="M2" s="25"/>
-      <c r="N2" s="100" t="s">
+      <c r="N2" s="88" t="s">
         <v>67</v>
       </c>
-      <c r="O2" s="87"/>
-      <c r="P2" s="87"/>
-      <c r="Q2" s="87"/>
-      <c r="R2" s="99"/>
+      <c r="O2" s="86"/>
+      <c r="P2" s="86"/>
+      <c r="Q2" s="86"/>
+      <c r="R2" s="87"/>
       <c r="S2" s="26"/>
-      <c r="T2" s="86" t="s">
+      <c r="T2" s="85" t="s">
         <v>66</v>
       </c>
-      <c r="U2" s="87"/>
-      <c r="V2" s="99"/>
-      <c r="W2" s="100" t="s">
+      <c r="U2" s="86"/>
+      <c r="V2" s="87"/>
+      <c r="W2" s="88" t="s">
         <v>65</v>
       </c>
-      <c r="X2" s="87"/>
-      <c r="Y2" s="87"/>
-      <c r="Z2" s="86" t="s">
+      <c r="X2" s="86"/>
+      <c r="Y2" s="86"/>
+      <c r="Z2" s="85" t="s">
         <v>64</v>
       </c>
-      <c r="AA2" s="87"/>
-      <c r="AB2" s="87"/>
-      <c r="AC2" s="86" t="s">
+      <c r="AA2" s="86"/>
+      <c r="AB2" s="86"/>
+      <c r="AC2" s="85" t="s">
         <v>63</v>
       </c>
-      <c r="AD2" s="87"/>
-      <c r="AE2" s="87"/>
+      <c r="AD2" s="86"/>
+      <c r="AE2" s="86"/>
     </row>
     <row r="3" spans="1:31" ht="13">
       <c r="A3" s="27"/>
@@ -3186,17 +3183,17 @@
       <c r="I3" s="28"/>
       <c r="J3" s="28"/>
       <c r="K3" s="29"/>
-      <c r="L3" s="88" t="s">
+      <c r="L3" s="94" t="s">
         <v>68</v>
       </c>
-      <c r="M3" s="89"/>
-      <c r="N3" s="89"/>
-      <c r="O3" s="89"/>
-      <c r="P3" s="89"/>
-      <c r="Q3" s="89"/>
-      <c r="R3" s="89"/>
-      <c r="S3" s="89"/>
-      <c r="T3" s="90"/>
+      <c r="M3" s="95"/>
+      <c r="N3" s="95"/>
+      <c r="O3" s="95"/>
+      <c r="P3" s="95"/>
+      <c r="Q3" s="95"/>
+      <c r="R3" s="95"/>
+      <c r="S3" s="95"/>
+      <c r="T3" s="96"/>
       <c r="U3" s="30"/>
       <c r="V3" s="28"/>
       <c r="W3" s="28"/>
@@ -3221,15 +3218,15 @@
       <c r="I4" s="35"/>
       <c r="J4" s="35"/>
       <c r="K4" s="36"/>
-      <c r="L4" s="91"/>
-      <c r="M4" s="81"/>
-      <c r="N4" s="81"/>
-      <c r="O4" s="81"/>
-      <c r="P4" s="81"/>
-      <c r="Q4" s="81"/>
-      <c r="R4" s="81"/>
-      <c r="S4" s="81"/>
-      <c r="T4" s="92"/>
+      <c r="L4" s="97"/>
+      <c r="M4" s="84"/>
+      <c r="N4" s="84"/>
+      <c r="O4" s="84"/>
+      <c r="P4" s="84"/>
+      <c r="Q4" s="84"/>
+      <c r="R4" s="84"/>
+      <c r="S4" s="84"/>
+      <c r="T4" s="90"/>
       <c r="U4" s="37"/>
       <c r="V4" s="23"/>
       <c r="W4" s="23"/>
@@ -3254,15 +3251,15 @@
       <c r="I5" s="35"/>
       <c r="J5" s="35"/>
       <c r="K5" s="36"/>
-      <c r="L5" s="93"/>
-      <c r="M5" s="94"/>
-      <c r="N5" s="94"/>
-      <c r="O5" s="94"/>
-      <c r="P5" s="94"/>
-      <c r="Q5" s="94"/>
-      <c r="R5" s="94"/>
-      <c r="S5" s="94"/>
-      <c r="T5" s="95"/>
+      <c r="L5" s="98"/>
+      <c r="M5" s="99"/>
+      <c r="N5" s="99"/>
+      <c r="O5" s="99"/>
+      <c r="P5" s="99"/>
+      <c r="Q5" s="99"/>
+      <c r="R5" s="99"/>
+      <c r="S5" s="99"/>
+      <c r="T5" s="100"/>
       <c r="U5" s="37"/>
       <c r="V5" s="23"/>
       <c r="W5" s="23"/>
@@ -3276,9 +3273,9 @@
       <c r="AE5" s="31"/>
     </row>
     <row r="6" spans="1:31" ht="15.5">
-      <c r="A6" s="97"/>
-      <c r="B6" s="81"/>
-      <c r="C6" s="92"/>
+      <c r="A6" s="89"/>
+      <c r="B6" s="84"/>
+      <c r="C6" s="90"/>
       <c r="D6" s="26"/>
       <c r="E6" s="42"/>
       <c r="F6" s="21"/>
@@ -3294,12 +3291,12 @@
       </c>
       <c r="O6" s="47">
         <f ca="1">R6</f>
-        <v>57</v>
+        <v>14</v>
       </c>
       <c r="Q6" s="47"/>
       <c r="R6" s="48">
         <f ca="1">ROUND(RAND()*COUNT(Criteria!A2:A59),0) + 1</f>
-        <v>57</v>
+        <v>14</v>
       </c>
       <c r="S6" s="28"/>
       <c r="T6" s="28" t="s">
@@ -3313,9 +3310,9 @@
       <c r="Z6" s="21"/>
       <c r="AA6" s="42"/>
       <c r="AB6" s="49"/>
-      <c r="AC6" s="85"/>
-      <c r="AD6" s="81"/>
-      <c r="AE6" s="81"/>
+      <c r="AC6" s="101"/>
+      <c r="AD6" s="84"/>
+      <c r="AE6" s="84"/>
     </row>
     <row r="7" spans="1:31" ht="13">
       <c r="A7" s="50"/>
@@ -3331,14 +3328,14 @@
       <c r="K7" s="35"/>
       <c r="L7" s="35"/>
       <c r="M7" s="35"/>
-      <c r="N7" s="96" t="str">
+      <c r="N7" s="102" t="str">
         <f ca="1">VLOOKUP(O6,Criteria!A2:B59,2,TRUE)</f>
-        <v>Has EEPROM (most wins)</v>
-      </c>
-      <c r="O7" s="81"/>
-      <c r="P7" s="81"/>
-      <c r="Q7" s="81"/>
-      <c r="R7" s="81"/>
+        <v xml:space="preserve">Has on-board programmer </v>
+      </c>
+      <c r="O7" s="84"/>
+      <c r="P7" s="84"/>
+      <c r="Q7" s="84"/>
+      <c r="R7" s="84"/>
       <c r="S7" s="23"/>
       <c r="T7" s="52" t="s">
         <v>70</v>
@@ -3369,11 +3366,11 @@
       <c r="K8" s="23"/>
       <c r="L8" s="23"/>
       <c r="M8" s="23"/>
-      <c r="N8" s="81"/>
-      <c r="O8" s="81"/>
-      <c r="P8" s="81"/>
-      <c r="Q8" s="81"/>
-      <c r="R8" s="81"/>
+      <c r="N8" s="84"/>
+      <c r="O8" s="84"/>
+      <c r="P8" s="84"/>
+      <c r="Q8" s="84"/>
+      <c r="R8" s="84"/>
       <c r="S8" s="23"/>
       <c r="T8" s="23"/>
       <c r="U8" s="23"/>
@@ -3402,11 +3399,11 @@
       <c r="K9" s="23"/>
       <c r="L9" s="23"/>
       <c r="M9" s="23"/>
-      <c r="N9" s="81"/>
-      <c r="O9" s="81"/>
-      <c r="P9" s="81"/>
-      <c r="Q9" s="81"/>
-      <c r="R9" s="81"/>
+      <c r="N9" s="84"/>
+      <c r="O9" s="84"/>
+      <c r="P9" s="84"/>
+      <c r="Q9" s="84"/>
+      <c r="R9" s="84"/>
       <c r="S9" s="23"/>
       <c r="T9" s="23"/>
       <c r="U9" s="23"/>
@@ -3425,9 +3422,9 @@
       <c r="A10" s="50"/>
       <c r="B10" s="50"/>
       <c r="C10" s="50"/>
-      <c r="D10" s="82"/>
-      <c r="E10" s="81"/>
-      <c r="F10" s="92"/>
+      <c r="D10" s="91"/>
+      <c r="E10" s="84"/>
+      <c r="F10" s="90"/>
       <c r="G10" s="26"/>
       <c r="H10" s="42"/>
       <c r="I10" s="21"/>
@@ -3435,11 +3432,11 @@
       <c r="K10" s="23"/>
       <c r="L10" s="23"/>
       <c r="M10" s="23"/>
-      <c r="N10" s="81"/>
-      <c r="O10" s="81"/>
-      <c r="P10" s="81"/>
-      <c r="Q10" s="81"/>
-      <c r="R10" s="81"/>
+      <c r="N10" s="84"/>
+      <c r="O10" s="84"/>
+      <c r="P10" s="84"/>
+      <c r="Q10" s="84"/>
+      <c r="R10" s="84"/>
       <c r="S10" s="23"/>
       <c r="T10" s="23"/>
       <c r="U10" s="23"/>
@@ -3447,9 +3444,9 @@
       <c r="W10" s="21"/>
       <c r="X10" s="42"/>
       <c r="Y10" s="49"/>
-      <c r="Z10" s="80"/>
-      <c r="AA10" s="81"/>
-      <c r="AB10" s="81"/>
+      <c r="Z10" s="83"/>
+      <c r="AA10" s="84"/>
+      <c r="AB10" s="84"/>
       <c r="AC10" s="54"/>
       <c r="AD10" s="54"/>
       <c r="AE10" s="54"/>
@@ -3467,11 +3464,11 @@
       <c r="K11" s="23"/>
       <c r="L11" s="23"/>
       <c r="M11" s="23"/>
-      <c r="N11" s="81"/>
-      <c r="O11" s="81"/>
-      <c r="P11" s="81"/>
-      <c r="Q11" s="81"/>
-      <c r="R11" s="81"/>
+      <c r="N11" s="84"/>
+      <c r="O11" s="84"/>
+      <c r="P11" s="84"/>
+      <c r="Q11" s="84"/>
+      <c r="R11" s="84"/>
       <c r="S11" s="23"/>
       <c r="T11" s="23"/>
       <c r="U11" s="23"/>
@@ -3500,11 +3497,11 @@
       <c r="K12" s="23"/>
       <c r="L12" s="23"/>
       <c r="M12" s="23"/>
-      <c r="N12" s="81"/>
-      <c r="O12" s="81"/>
-      <c r="P12" s="81"/>
-      <c r="Q12" s="81"/>
-      <c r="R12" s="81"/>
+      <c r="N12" s="84"/>
+      <c r="O12" s="84"/>
+      <c r="P12" s="84"/>
+      <c r="Q12" s="84"/>
+      <c r="R12" s="84"/>
       <c r="S12" s="23"/>
       <c r="T12" s="23"/>
       <c r="U12" s="23"/>
@@ -3532,11 +3529,11 @@
       <c r="K13" s="23"/>
       <c r="L13" s="23"/>
       <c r="M13" s="23"/>
-      <c r="N13" s="81"/>
-      <c r="O13" s="81"/>
-      <c r="P13" s="81"/>
-      <c r="Q13" s="81"/>
-      <c r="R13" s="81"/>
+      <c r="N13" s="84"/>
+      <c r="O13" s="84"/>
+      <c r="P13" s="84"/>
+      <c r="Q13" s="84"/>
+      <c r="R13" s="84"/>
       <c r="S13" s="23"/>
       <c r="T13" s="23"/>
       <c r="U13" s="23"/>
@@ -3552,9 +3549,9 @@
       <c r="AE13" s="31"/>
     </row>
     <row r="14" spans="1:31" ht="13">
-      <c r="A14" s="97"/>
-      <c r="B14" s="81"/>
-      <c r="C14" s="92"/>
+      <c r="A14" s="89"/>
+      <c r="B14" s="84"/>
+      <c r="C14" s="90"/>
       <c r="D14" s="26"/>
       <c r="E14" s="42"/>
       <c r="F14" s="49"/>
@@ -3565,11 +3562,11 @@
       <c r="K14" s="23"/>
       <c r="L14" s="23"/>
       <c r="M14" s="23"/>
-      <c r="N14" s="81"/>
-      <c r="O14" s="81"/>
-      <c r="P14" s="81"/>
-      <c r="Q14" s="81"/>
-      <c r="R14" s="81"/>
+      <c r="N14" s="84"/>
+      <c r="O14" s="84"/>
+      <c r="P14" s="84"/>
+      <c r="Q14" s="84"/>
+      <c r="R14" s="84"/>
       <c r="S14" s="23"/>
       <c r="T14" s="23"/>
       <c r="U14" s="23"/>
@@ -3580,9 +3577,9 @@
       <c r="Z14" s="26"/>
       <c r="AA14" s="42"/>
       <c r="AB14" s="49"/>
-      <c r="AC14" s="85"/>
-      <c r="AD14" s="81"/>
-      <c r="AE14" s="81"/>
+      <c r="AC14" s="101"/>
+      <c r="AD14" s="84"/>
+      <c r="AE14" s="84"/>
     </row>
     <row r="15" spans="1:31" ht="13">
       <c r="A15" s="50"/>
@@ -3597,11 +3594,11 @@
       <c r="K15" s="23"/>
       <c r="L15" s="23"/>
       <c r="M15" s="23"/>
-      <c r="N15" s="81"/>
-      <c r="O15" s="81"/>
-      <c r="P15" s="81"/>
-      <c r="Q15" s="81"/>
-      <c r="R15" s="81"/>
+      <c r="N15" s="84"/>
+      <c r="O15" s="84"/>
+      <c r="P15" s="84"/>
+      <c r="Q15" s="84"/>
+      <c r="R15" s="84"/>
       <c r="S15" s="23"/>
       <c r="T15" s="23"/>
       <c r="U15" s="23"/>
@@ -3630,11 +3627,11 @@
       <c r="K16" s="23"/>
       <c r="L16" s="23"/>
       <c r="M16" s="23"/>
-      <c r="N16" s="81"/>
-      <c r="O16" s="81"/>
-      <c r="P16" s="81"/>
-      <c r="Q16" s="81"/>
-      <c r="R16" s="81"/>
+      <c r="N16" s="84"/>
+      <c r="O16" s="84"/>
+      <c r="P16" s="84"/>
+      <c r="Q16" s="84"/>
+      <c r="R16" s="84"/>
       <c r="S16" s="23"/>
       <c r="T16" s="23"/>
       <c r="U16" s="23"/>
@@ -3662,11 +3659,11 @@
       <c r="K17" s="23"/>
       <c r="L17" s="23"/>
       <c r="M17" s="23"/>
-      <c r="N17" s="81"/>
-      <c r="O17" s="81"/>
-      <c r="P17" s="81"/>
-      <c r="Q17" s="81"/>
-      <c r="R17" s="81"/>
+      <c r="N17" s="84"/>
+      <c r="O17" s="84"/>
+      <c r="P17" s="84"/>
+      <c r="Q17" s="84"/>
+      <c r="R17" s="84"/>
       <c r="S17" s="23"/>
       <c r="T17" s="23"/>
       <c r="U17" s="23"/>
@@ -3688,9 +3685,9 @@
       <c r="D18" s="23"/>
       <c r="E18" s="23"/>
       <c r="F18" s="23"/>
-      <c r="G18" s="101"/>
-      <c r="H18" s="81"/>
-      <c r="I18" s="92"/>
+      <c r="G18" s="92"/>
+      <c r="H18" s="84"/>
+      <c r="I18" s="90"/>
       <c r="J18" s="26"/>
       <c r="K18" s="42"/>
       <c r="L18" s="21"/>
@@ -3704,9 +3701,9 @@
       <c r="T18" s="21"/>
       <c r="U18" s="42"/>
       <c r="V18" s="49"/>
-      <c r="W18" s="80"/>
-      <c r="X18" s="81"/>
-      <c r="Y18" s="81"/>
+      <c r="W18" s="83"/>
+      <c r="X18" s="84"/>
+      <c r="Y18" s="84"/>
       <c r="Z18" s="23"/>
       <c r="AA18" s="23"/>
       <c r="AB18" s="23"/>
@@ -3809,9 +3806,9 @@
       <c r="AE21" s="31"/>
     </row>
     <row r="22" spans="1:31" ht="13">
-      <c r="A22" s="97"/>
-      <c r="B22" s="81"/>
-      <c r="C22" s="92"/>
+      <c r="A22" s="89"/>
+      <c r="B22" s="84"/>
+      <c r="C22" s="90"/>
       <c r="D22" s="26"/>
       <c r="E22" s="42"/>
       <c r="F22" s="21"/>
@@ -3837,9 +3834,9 @@
       <c r="Z22" s="21"/>
       <c r="AA22" s="42"/>
       <c r="AB22" s="49"/>
-      <c r="AC22" s="85"/>
-      <c r="AD22" s="81"/>
-      <c r="AE22" s="81"/>
+      <c r="AC22" s="101"/>
+      <c r="AD22" s="84"/>
+      <c r="AE22" s="84"/>
     </row>
     <row r="23" spans="1:31" ht="13">
       <c r="A23" s="50"/>
@@ -3940,9 +3937,9 @@
       <c r="A26" s="50"/>
       <c r="B26" s="50"/>
       <c r="C26" s="50"/>
-      <c r="D26" s="82"/>
-      <c r="E26" s="81"/>
-      <c r="F26" s="92"/>
+      <c r="D26" s="91"/>
+      <c r="E26" s="84"/>
+      <c r="F26" s="90"/>
       <c r="G26" s="26"/>
       <c r="H26" s="42"/>
       <c r="I26" s="49"/>
@@ -3962,9 +3959,9 @@
       <c r="W26" s="26"/>
       <c r="X26" s="42"/>
       <c r="Y26" s="49"/>
-      <c r="Z26" s="80"/>
-      <c r="AA26" s="81"/>
-      <c r="AB26" s="81"/>
+      <c r="Z26" s="83"/>
+      <c r="AA26" s="84"/>
+      <c r="AB26" s="84"/>
       <c r="AC26" s="54"/>
       <c r="AD26" s="54"/>
       <c r="AE26" s="54"/>
@@ -4066,9 +4063,9 @@
       <c r="AE29" s="31"/>
     </row>
     <row r="30" spans="1:31" ht="13">
-      <c r="A30" s="97"/>
-      <c r="B30" s="81"/>
-      <c r="C30" s="92"/>
+      <c r="A30" s="89"/>
+      <c r="B30" s="84"/>
+      <c r="C30" s="90"/>
       <c r="D30" s="26"/>
       <c r="E30" s="42"/>
       <c r="F30" s="49"/>
@@ -4094,9 +4091,9 @@
       <c r="Z30" s="26"/>
       <c r="AA30" s="42"/>
       <c r="AB30" s="49"/>
-      <c r="AC30" s="85"/>
-      <c r="AD30" s="81"/>
-      <c r="AE30" s="81"/>
+      <c r="AC30" s="101"/>
+      <c r="AD30" s="84"/>
+      <c r="AE30" s="84"/>
     </row>
     <row r="31" spans="1:31" ht="13">
       <c r="A31" s="50"/>
@@ -4204,9 +4201,9 @@
       <c r="G34" s="23"/>
       <c r="H34" s="23"/>
       <c r="I34" s="23"/>
-      <c r="J34" s="82"/>
-      <c r="K34" s="81"/>
-      <c r="L34" s="92"/>
+      <c r="J34" s="91"/>
+      <c r="K34" s="84"/>
+      <c r="L34" s="90"/>
       <c r="M34" s="26"/>
       <c r="N34" s="42"/>
       <c r="O34" s="21"/>
@@ -4214,9 +4211,9 @@
       <c r="Q34" s="21"/>
       <c r="R34" s="42"/>
       <c r="S34" s="49"/>
-      <c r="T34" s="80"/>
-      <c r="U34" s="81"/>
-      <c r="V34" s="81"/>
+      <c r="T34" s="83"/>
+      <c r="U34" s="84"/>
+      <c r="V34" s="84"/>
       <c r="W34" s="23"/>
       <c r="X34" s="23"/>
       <c r="Y34" s="23"/>
@@ -4324,9 +4321,9 @@
       <c r="AE37" s="69"/>
     </row>
     <row r="38" spans="1:31" ht="13">
-      <c r="A38" s="98"/>
-      <c r="B38" s="81"/>
-      <c r="C38" s="92"/>
+      <c r="A38" s="93"/>
+      <c r="B38" s="84"/>
+      <c r="C38" s="90"/>
       <c r="D38" s="26"/>
       <c r="E38" s="42"/>
       <c r="F38" s="21"/>
@@ -4354,9 +4351,9 @@
       <c r="Z38" s="21"/>
       <c r="AA38" s="42"/>
       <c r="AB38" s="49"/>
-      <c r="AC38" s="83"/>
-      <c r="AD38" s="81"/>
-      <c r="AE38" s="81"/>
+      <c r="AC38" s="103"/>
+      <c r="AD38" s="84"/>
+      <c r="AE38" s="84"/>
     </row>
     <row r="39" spans="1:31" ht="13">
       <c r="A39" s="62"/>
@@ -4457,9 +4454,9 @@
       <c r="A42" s="62"/>
       <c r="B42" s="62"/>
       <c r="C42" s="62"/>
-      <c r="D42" s="82"/>
-      <c r="E42" s="81"/>
-      <c r="F42" s="92"/>
+      <c r="D42" s="91"/>
+      <c r="E42" s="84"/>
+      <c r="F42" s="90"/>
       <c r="G42" s="26"/>
       <c r="H42" s="42"/>
       <c r="I42" s="21"/>
@@ -4479,9 +4476,9 @@
       <c r="W42" s="21"/>
       <c r="X42" s="42"/>
       <c r="Y42" s="49"/>
-      <c r="Z42" s="80"/>
-      <c r="AA42" s="81"/>
-      <c r="AB42" s="81"/>
+      <c r="Z42" s="83"/>
+      <c r="AA42" s="84"/>
+      <c r="AB42" s="84"/>
       <c r="AC42" s="63"/>
       <c r="AD42" s="63"/>
       <c r="AE42" s="63"/>
@@ -4582,9 +4579,9 @@
       <c r="AE45" s="69"/>
     </row>
     <row r="46" spans="1:31" ht="13">
-      <c r="A46" s="98"/>
-      <c r="B46" s="81"/>
-      <c r="C46" s="92"/>
+      <c r="A46" s="93"/>
+      <c r="B46" s="84"/>
+      <c r="C46" s="90"/>
       <c r="D46" s="26"/>
       <c r="E46" s="42"/>
       <c r="F46" s="49"/>
@@ -4610,9 +4607,9 @@
       <c r="Z46" s="26"/>
       <c r="AA46" s="42"/>
       <c r="AB46" s="49"/>
-      <c r="AC46" s="83"/>
-      <c r="AD46" s="81"/>
-      <c r="AE46" s="81"/>
+      <c r="AC46" s="103"/>
+      <c r="AD46" s="84"/>
+      <c r="AE46" s="84"/>
     </row>
     <row r="47" spans="1:31" ht="13">
       <c r="A47" s="62"/>
@@ -4715,9 +4712,9 @@
       <c r="D50" s="23"/>
       <c r="E50" s="23"/>
       <c r="F50" s="23"/>
-      <c r="G50" s="82"/>
-      <c r="H50" s="81"/>
-      <c r="I50" s="92"/>
+      <c r="G50" s="91"/>
+      <c r="H50" s="84"/>
+      <c r="I50" s="90"/>
       <c r="J50" s="26"/>
       <c r="K50" s="42"/>
       <c r="L50" s="49"/>
@@ -4731,9 +4728,9 @@
       <c r="T50" s="26"/>
       <c r="U50" s="42"/>
       <c r="V50" s="49"/>
-      <c r="W50" s="80"/>
-      <c r="X50" s="81"/>
-      <c r="Y50" s="81"/>
+      <c r="W50" s="83"/>
+      <c r="X50" s="84"/>
+      <c r="Y50" s="84"/>
       <c r="Z50" s="23"/>
       <c r="AA50" s="23"/>
       <c r="AB50" s="23"/>
@@ -4819,9 +4816,9 @@
       <c r="L53" s="75"/>
       <c r="M53" s="23"/>
       <c r="N53" s="61"/>
-      <c r="O53" s="84"/>
-      <c r="P53" s="81"/>
-      <c r="Q53" s="81"/>
+      <c r="O53" s="104"/>
+      <c r="P53" s="84"/>
+      <c r="Q53" s="84"/>
       <c r="R53" s="61"/>
       <c r="S53" s="23"/>
       <c r="T53" s="75"/>
@@ -4837,9 +4834,9 @@
       <c r="AE53" s="69"/>
     </row>
     <row r="54" spans="1:31" ht="13">
-      <c r="A54" s="98"/>
-      <c r="B54" s="81"/>
-      <c r="C54" s="92"/>
+      <c r="A54" s="93"/>
+      <c r="B54" s="84"/>
+      <c r="C54" s="90"/>
       <c r="D54" s="26"/>
       <c r="E54" s="42"/>
       <c r="F54" s="21"/>
@@ -4865,9 +4862,9 @@
       <c r="Z54" s="21"/>
       <c r="AA54" s="42"/>
       <c r="AB54" s="49"/>
-      <c r="AC54" s="83"/>
-      <c r="AD54" s="81"/>
-      <c r="AE54" s="81"/>
+      <c r="AC54" s="103"/>
+      <c r="AD54" s="84"/>
+      <c r="AE54" s="84"/>
     </row>
     <row r="55" spans="1:31" ht="13">
       <c r="A55" s="62"/>
@@ -4913,13 +4910,13 @@
       <c r="J56" s="37"/>
       <c r="K56" s="23"/>
       <c r="L56" s="77"/>
-      <c r="M56" s="82"/>
-      <c r="N56" s="81"/>
-      <c r="O56" s="81"/>
+      <c r="M56" s="91"/>
+      <c r="N56" s="84"/>
+      <c r="O56" s="84"/>
       <c r="P56" s="23"/>
-      <c r="Q56" s="82"/>
-      <c r="R56" s="81"/>
-      <c r="S56" s="81"/>
+      <c r="Q56" s="91"/>
+      <c r="R56" s="84"/>
+      <c r="S56" s="84"/>
       <c r="T56" s="78"/>
       <c r="U56" s="23"/>
       <c r="V56" s="40"/>
@@ -4967,9 +4964,9 @@
       <c r="A58" s="62"/>
       <c r="B58" s="62"/>
       <c r="C58" s="62"/>
-      <c r="D58" s="82"/>
-      <c r="E58" s="81"/>
-      <c r="F58" s="92"/>
+      <c r="D58" s="91"/>
+      <c r="E58" s="84"/>
+      <c r="F58" s="90"/>
       <c r="G58" s="26"/>
       <c r="H58" s="42"/>
       <c r="I58" s="49"/>
@@ -4989,9 +4986,9 @@
       <c r="W58" s="26"/>
       <c r="X58" s="42"/>
       <c r="Y58" s="49"/>
-      <c r="Z58" s="80"/>
-      <c r="AA58" s="81"/>
-      <c r="AB58" s="81"/>
+      <c r="Z58" s="83"/>
+      <c r="AA58" s="84"/>
+      <c r="AB58" s="84"/>
       <c r="AC58" s="63"/>
       <c r="AD58" s="63"/>
       <c r="AE58" s="63"/>
@@ -5040,13 +5037,13 @@
       <c r="J60" s="23"/>
       <c r="K60" s="23"/>
       <c r="L60" s="77"/>
-      <c r="M60" s="82"/>
-      <c r="N60" s="81"/>
-      <c r="O60" s="81"/>
+      <c r="M60" s="91"/>
+      <c r="N60" s="84"/>
+      <c r="O60" s="84"/>
       <c r="P60" s="23"/>
-      <c r="Q60" s="82"/>
-      <c r="R60" s="81"/>
-      <c r="S60" s="81"/>
+      <c r="Q60" s="91"/>
+      <c r="R60" s="84"/>
+      <c r="S60" s="84"/>
       <c r="T60" s="78"/>
       <c r="U60" s="23"/>
       <c r="V60" s="23"/>
@@ -5091,9 +5088,9 @@
       <c r="AE61" s="69"/>
     </row>
     <row r="62" spans="1:31" ht="13">
-      <c r="A62" s="98"/>
-      <c r="B62" s="81"/>
-      <c r="C62" s="92"/>
+      <c r="A62" s="93"/>
+      <c r="B62" s="84"/>
+      <c r="C62" s="90"/>
       <c r="D62" s="26"/>
       <c r="E62" s="79"/>
       <c r="F62" s="49"/>
@@ -5119,9 +5116,9 @@
       <c r="Z62" s="26"/>
       <c r="AA62" s="42"/>
       <c r="AB62" s="49"/>
-      <c r="AC62" s="83"/>
-      <c r="AD62" s="81"/>
-      <c r="AE62" s="81"/>
+      <c r="AC62" s="103"/>
+      <c r="AD62" s="84"/>
+      <c r="AE62" s="84"/>
     </row>
     <row r="63" spans="1:31" ht="13">
       <c r="A63" s="62"/>
@@ -5252,41 +5249,6 @@
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="W18:Y18"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="N2:R2"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="A38:C38"/>
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="A54:C54"/>
-    <mergeCell ref="A62:C62"/>
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="J34:L34"/>
-    <mergeCell ref="D42:F42"/>
-    <mergeCell ref="G50:I50"/>
-    <mergeCell ref="D58:F58"/>
-    <mergeCell ref="Z2:AB2"/>
-    <mergeCell ref="AC2:AE2"/>
-    <mergeCell ref="L3:T5"/>
-    <mergeCell ref="AC6:AE6"/>
-    <mergeCell ref="N7:R17"/>
-    <mergeCell ref="Z10:AB10"/>
-    <mergeCell ref="AC14:AE14"/>
-    <mergeCell ref="T2:V2"/>
-    <mergeCell ref="W2:Y2"/>
-    <mergeCell ref="AC22:AE22"/>
-    <mergeCell ref="Z26:AB26"/>
-    <mergeCell ref="AC30:AE30"/>
-    <mergeCell ref="T34:V34"/>
-    <mergeCell ref="AC38:AE38"/>
     <mergeCell ref="Z42:AB42"/>
     <mergeCell ref="M60:O60"/>
     <mergeCell ref="Q60:S60"/>
@@ -5298,6 +5260,41 @@
     <mergeCell ref="M56:O56"/>
     <mergeCell ref="Q56:S56"/>
     <mergeCell ref="Z58:AB58"/>
+    <mergeCell ref="AC22:AE22"/>
+    <mergeCell ref="Z26:AB26"/>
+    <mergeCell ref="AC30:AE30"/>
+    <mergeCell ref="T34:V34"/>
+    <mergeCell ref="AC38:AE38"/>
+    <mergeCell ref="Z2:AB2"/>
+    <mergeCell ref="AC2:AE2"/>
+    <mergeCell ref="L3:T5"/>
+    <mergeCell ref="AC6:AE6"/>
+    <mergeCell ref="N7:R17"/>
+    <mergeCell ref="Z10:AB10"/>
+    <mergeCell ref="AC14:AE14"/>
+    <mergeCell ref="T2:V2"/>
+    <mergeCell ref="W2:Y2"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="A54:C54"/>
+    <mergeCell ref="A62:C62"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="J34:L34"/>
+    <mergeCell ref="D42:F42"/>
+    <mergeCell ref="G50:I50"/>
+    <mergeCell ref="D58:F58"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="A38:C38"/>
+    <mergeCell ref="W18:Y18"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="N2:R2"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A14:C14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>